<commit_message>
resolved error when opening the doc
</commit_message>
<xml_diff>
--- a/doc/checkers-inventory/eProcurement conceptual model checkers inventory.xlsx
+++ b/doc/checkers-inventory/eProcurement conceptual model checkers inventory.xlsx
@@ -13,12 +13,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="210">
   <si>
     <t>Inventory of checkers for the UML model conventions</t>
   </si>
   <si>
-    <t>Date</t>
+    <t>Last updated</t>
   </si>
   <si>
     <t>Note: a category can inherit checkers from another category. For example, ‘association’ inheriting all checkers from the generic ‘connector’ is represented as ‘association-&gt;connector’. If no subcategory is provided then all the checkers are inherited, else if a subcategory is provided then the inheritance is limited to the checkers of that subcategory only (e.g. class -&gt; common, name). The variable names, surrounded by the dollar sign $, are used in the checker messages, e.g. $elementName$.</t>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>association-&gt;connector</t>
+  </si>
+  <si>
+    <t>inherits all from checkers in category connector</t>
   </si>
   <si>
     <t>see connector-name-27
@@ -141,16 +144,25 @@
     <t>class-&gt;common</t>
   </si>
   <si>
+    <t>inherits all from checkers in category common and subcategory name</t>
+  </si>
+  <si>
     <t>see common-name-1 to common-name-8 and common-name-57, common-name-58</t>
   </si>
   <si>
     <t>description</t>
   </si>
   <si>
+    <t>inherits all from checkers in category common and subcategory description</t>
+  </si>
+  <si>
     <t>see common-description-9</t>
   </si>
   <si>
     <t>stereotype</t>
+  </si>
+  <si>
+    <t>inherits all from checkers in category common and subcategory stereotype</t>
   </si>
   <si>
     <t>common-stereotype-10</t>
@@ -648,7 +660,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -672,8 +684,6 @@
     <font>
       <b/>
       <i/>
-      <color theme="1"/>
-      <name val="Arial"/>
     </font>
     <font>
       <i/>
@@ -690,7 +700,6 @@
     <font>
       <color rgb="FF000000"/>
     </font>
-    <font/>
   </fonts>
   <fills count="5">
     <fill>
@@ -754,7 +763,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -791,51 +800,49 @@
     <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="2" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="2" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="4" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1090,7 +1097,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="5">
-        <v>44086.0</v>
+        <v>44093.0</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="1"/>
@@ -1216,13 +1223,13 @@
       <c r="E9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="15" t="s">
         <v>19</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="16">
         <v>33.0</v>
       </c>
     </row>
@@ -1256,19 +1263,27 @@
     <row r="11">
       <c r="A11" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>association-&gt;connector--36</v>
+        <v>association-&gt;connector-inherits all from checkers in category connector-36</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16" t="s">
+      <c r="C11" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="17">
+      <c r="D11" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="16">
         <v>36.0</v>
       </c>
     </row>
@@ -1278,22 +1293,22 @@
         <v>class-name-14</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H12" s="13">
         <v>14.0</v>
@@ -1305,24 +1320,24 @@
         <v>class-attributes-15</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="17">
+        <v>35</v>
+      </c>
+      <c r="H13" s="16">
         <v>15.0</v>
       </c>
     </row>
@@ -1332,22 +1347,22 @@
         <v>class-connectors-16</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H14" s="13">
         <v>16.0</v>
@@ -1359,18 +1374,24 @@
         <v>class-&gt;common-name-11</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="17">
+        <v>28</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="16">
         <v>11.0</v>
       </c>
     </row>
@@ -1380,17 +1401,23 @@
         <v>class-&gt;common-description-12</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
+        <v>43</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>44</v>
+      </c>
       <c r="H16" s="13">
         <v>12.0</v>
       </c>
@@ -1401,18 +1428,24 @@
         <v>class-&gt;common-stereotype-13</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="17">
+        <v>46</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="16">
         <v>13.0</v>
       </c>
     </row>
@@ -1422,22 +1455,22 @@
         <v>class-attribute-name-21</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H18" s="13">
         <v>21.0</v>
@@ -1449,7 +1482,7 @@
         <v>class-attribute-multiplicity-22</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>16</v>
@@ -1458,15 +1491,15 @@
         <v>12</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="H19" s="17">
+        <v>54</v>
+      </c>
+      <c r="H19" s="16">
         <v>22.0</v>
       </c>
     </row>
@@ -1476,22 +1509,22 @@
         <v>class-attribute-type-23</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="22" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H20" s="13">
         <v>23.0</v>
@@ -1503,24 +1536,24 @@
         <v>class-attribute-type-24</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="H21" s="17">
+        <v>61</v>
+      </c>
+      <c r="H21" s="16">
         <v>24.0</v>
       </c>
     </row>
@@ -1530,22 +1563,22 @@
         <v>class-attribute-type-25</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H22" s="13">
         <v>25.0</v>
@@ -1557,24 +1590,24 @@
         <v>class-attribute-counter-part-65</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="H23" s="17">
+        <v>68</v>
+      </c>
+      <c r="H23" s="16">
         <v>65.0</v>
       </c>
     </row>
@@ -1584,17 +1617,23 @@
         <v>class-attribute-&gt;common-name-18</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
+        <v>28</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>41</v>
+      </c>
       <c r="H24" s="13">
         <v>18.0</v>
       </c>
@@ -1605,18 +1644,24 @@
         <v>class-attribute-&gt;common-description-19</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="17">
+        <v>43</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H25" s="16">
         <v>19.0</v>
       </c>
     </row>
@@ -1626,17 +1671,23 @@
         <v>class-attribute-&gt;common-stereotype-20</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
+        <v>46</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>47</v>
+      </c>
       <c r="H26" s="13">
         <v>20.0</v>
       </c>
@@ -1647,24 +1698,24 @@
         <v>common-name-1</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D27" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="H27" s="17">
+        <v>73</v>
+      </c>
+      <c r="H27" s="16">
         <v>1.0</v>
       </c>
     </row>
@@ -1674,22 +1725,22 @@
         <v>common-name-2</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="H28" s="13">
         <v>2.0</v>
@@ -1701,24 +1752,24 @@
         <v>common-name-3</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D29" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="H29" s="17">
+        <v>79</v>
+      </c>
+      <c r="H29" s="16">
         <v>3.0</v>
       </c>
     </row>
@@ -1728,22 +1779,22 @@
         <v>common-name-4</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="H30" s="13">
         <v>4.0</v>
@@ -1755,24 +1806,24 @@
         <v>common-name-5</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="H31" s="17">
+        <v>85</v>
+      </c>
+      <c r="H31" s="16">
         <v>5.0</v>
       </c>
     </row>
@@ -1782,22 +1833,22 @@
         <v>common-name-6</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="H32" s="13">
         <v>6.0</v>
@@ -1809,24 +1860,24 @@
         <v>common-name-7</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="H33" s="17">
+        <v>91</v>
+      </c>
+      <c r="H33" s="16">
         <v>7.0</v>
       </c>
     </row>
@@ -1836,22 +1887,22 @@
         <v>common-name-8</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="H34" s="13">
         <v>8.0</v>
@@ -1863,24 +1914,24 @@
         <v>common-description-9</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D35" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="G35" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="H35" s="17">
+        <v>97</v>
+      </c>
+      <c r="H35" s="16">
         <v>9.0</v>
       </c>
     </row>
@@ -1890,22 +1941,22 @@
         <v>common-stereotype-10</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="H36" s="13">
         <v>10.0</v>
@@ -1917,24 +1968,24 @@
         <v>common-name-57</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D37" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="H37" s="17">
+        <v>103</v>
+      </c>
+      <c r="H37" s="16">
         <v>57.0</v>
       </c>
     </row>
@@ -1944,22 +1995,22 @@
         <v>common-name-58</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="H38" s="13">
         <v>58.0</v>
@@ -1971,24 +2022,24 @@
         <v>connector-name-27</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D39" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="H39" s="17">
+        <v>110</v>
+      </c>
+      <c r="H39" s="16">
         <v>27.0</v>
       </c>
     </row>
@@ -1998,22 +2049,22 @@
         <v>connector-description-28</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D40" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F40" s="22" t="s">
-        <v>107</v>
+        <v>95</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>111</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="H40" s="13">
         <v>28.0</v>
@@ -2025,24 +2076,24 @@
         <v>connector-target-29</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D41" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="H41" s="17">
+        <v>116</v>
+      </c>
+      <c r="H41" s="16">
         <v>29.0</v>
       </c>
     </row>
@@ -2052,22 +2103,22 @@
         <v>connector-direction-31</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D42" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="H42" s="13">
         <v>31.0</v>
@@ -2079,7 +2130,7 @@
         <v>connector-multiplicity-32</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C43" s="15" t="s">
         <v>16</v>
@@ -2088,15 +2139,15 @@
         <v>17</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="F43" s="16" t="s">
-        <v>118</v>
+        <v>121</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>122</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="H43" s="17">
+        <v>123</v>
+      </c>
+      <c r="H43" s="16">
         <v>32.0</v>
       </c>
     </row>
@@ -2106,7 +2157,7 @@
         <v>connector-multiplicity-34</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C44" s="12" t="s">
         <v>16</v>
@@ -2115,13 +2166,13 @@
         <v>12</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="H44" s="13">
         <v>34.0</v>
@@ -2133,24 +2184,24 @@
         <v>connector-direction-63</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D45" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E45" s="15" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="H45" s="17">
+        <v>129</v>
+      </c>
+      <c r="H45" s="16">
         <v>63.0</v>
       </c>
     </row>
@@ -2160,22 +2211,22 @@
         <v>datatype-name-61</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="G46" s="12" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="H46" s="13">
         <v>61.0</v>
@@ -2187,18 +2238,24 @@
         <v>datatype-&gt;common-name-54</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D47" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="17">
+        <v>28</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G47" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H47" s="16">
         <v>54.0</v>
       </c>
     </row>
@@ -2208,17 +2265,23 @@
         <v>datatype-&gt;common-description-55</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="20"/>
+        <v>43</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F48" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G48" s="18" t="s">
+        <v>44</v>
+      </c>
       <c r="H48" s="13">
         <v>55.0</v>
       </c>
@@ -2229,18 +2292,24 @@
         <v>datatype-&gt;common-stereotype-56</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="17">
+        <v>46</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="G49" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H49" s="16">
         <v>56.0</v>
       </c>
     </row>
@@ -2250,22 +2319,22 @@
         <v>dependency-direction-64</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D50" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="G50" s="12" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="H50" s="13">
         <v>64.0</v>
@@ -2274,19 +2343,27 @@
     <row r="51">
       <c r="A51" s="14" t="str">
         <f t="shared" si="1"/>
-        <v>dependency-&gt;connector--37</v>
+        <v>dependency-&gt;connector-inherits all from checkers in category connector-37</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="C51" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
-      <c r="H51" s="17">
+      <c r="D51" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G51" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H51" s="16">
         <v>37.0</v>
       </c>
     </row>
@@ -2296,22 +2373,22 @@
         <v>enum-attribute-name-51</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D52" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F52" s="12" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="G52" s="12" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H52" s="13">
         <v>51.0</v>
@@ -2323,24 +2400,24 @@
         <v>enum-attribute-name-52</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D53" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="H53" s="17">
+        <v>146</v>
+      </c>
+      <c r="H53" s="16">
         <v>52.0</v>
       </c>
     </row>
@@ -2350,22 +2427,22 @@
         <v>enum-attribute-name-60</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="F54" s="12" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="G54" s="12" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="H54" s="13">
         <v>60.0</v>
@@ -2377,18 +2454,20 @@
         <v>enum-attribute-&gt;common-description-53</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E55" s="15"/>
-      <c r="F55" s="23"/>
-      <c r="G55" s="23"/>
-      <c r="H55" s="17">
+        <v>45</v>
+      </c>
+      <c r="E55" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="16">
         <v>53.0</v>
       </c>
     </row>
@@ -2398,22 +2477,22 @@
         <v>enumeration-name-59</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F56" s="12" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="G56" s="12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H56" s="13">
         <v>59.0</v>
@@ -2425,18 +2504,24 @@
         <v>enumeration-&gt;common-name-48</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D57" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E57" s="18"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
-      <c r="H57" s="17">
+        <v>28</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E57" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G57" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H57" s="16">
         <v>48.0</v>
       </c>
     </row>
@@ -2446,17 +2531,23 @@
         <v>enumeration-&gt;common-stereotype-49</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C58" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="20"/>
+        <v>46</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E58" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="F58" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G58" s="18" t="s">
+        <v>47</v>
+      </c>
       <c r="H58" s="13">
         <v>49.0</v>
       </c>
@@ -2467,18 +2558,24 @@
         <v>enumeration-&gt;common-description-50</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D59" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="18"/>
-      <c r="H59" s="17">
+        <v>43</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E59" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F59" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G59" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H59" s="16">
         <v>50.0</v>
       </c>
     </row>
@@ -2488,22 +2585,22 @@
         <v>generalisation-hierarchy-38</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C60" s="12" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D60" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="F60" s="12" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="G60" s="12" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="H60" s="13">
         <v>38.0</v>
@@ -2515,24 +2612,24 @@
         <v>generalisation-hierarchy-39</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D61" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="F61" s="15" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="G61" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="H61" s="17">
+        <v>162</v>
+      </c>
+      <c r="H61" s="16">
         <v>39.0</v>
       </c>
     </row>
@@ -2542,7 +2639,7 @@
         <v>generalisation-multiplicity-40</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C62" s="12" t="s">
         <v>16</v>
@@ -2551,13 +2648,13 @@
         <v>17</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="F62" s="12" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="G62" s="12" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H62" s="13">
         <v>40.0</v>
@@ -2569,24 +2666,24 @@
         <v>generalisation-name-41</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D63" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E63" s="16" t="s">
-        <v>162</v>
+      <c r="E63" s="15" t="s">
+        <v>166</v>
       </c>
       <c r="F63" s="15" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="G63" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="H63" s="17">
+        <v>168</v>
+      </c>
+      <c r="H63" s="16">
         <v>41.0</v>
       </c>
     </row>
@@ -2596,22 +2693,22 @@
         <v>generalisation-name-42</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D64" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E64" s="22" t="s">
-        <v>165</v>
+      <c r="E64" s="12" t="s">
+        <v>169</v>
       </c>
       <c r="F64" s="12" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="G64" s="12" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="H64" s="13">
         <v>42.0</v>
@@ -2623,24 +2720,24 @@
         <v>generalisation-direction-62</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D65" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F65" s="15" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="G65" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="H65" s="17">
+        <v>173</v>
+      </c>
+      <c r="H65" s="16">
         <v>62.0</v>
       </c>
     </row>
@@ -2650,22 +2747,22 @@
         <v>package-name-43</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D66" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="F66" s="12" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="G66" s="12" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="H66" s="13">
         <v>43.0</v>
@@ -2677,24 +2774,24 @@
         <v>package-name-46</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D67" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E67" s="15" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="F67" s="15" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="H67" s="17">
+        <v>179</v>
+      </c>
+      <c r="H67" s="16">
         <v>46.0</v>
       </c>
     </row>
@@ -2704,22 +2801,22 @@
         <v>package-owned elements-47</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D68" s="12" t="s">
         <v>17</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="F68" s="12" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="G68" s="12" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="H68" s="13">
         <v>47.0</v>
@@ -2731,18 +2828,24 @@
         <v>package-&gt;common-description-44</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D69" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E69" s="18"/>
-      <c r="F69" s="18"/>
-      <c r="G69" s="18"/>
-      <c r="H69" s="17">
+        <v>43</v>
+      </c>
+      <c r="D69" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E69" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F69" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G69" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H69" s="16">
         <v>44.0</v>
       </c>
       <c r="I69" s="2"/>
@@ -2771,17 +2874,23 @@
         <v>package-&gt;common-stereotype-45</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C70" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D70" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E70" s="20"/>
-      <c r="F70" s="20"/>
-      <c r="G70" s="20"/>
+        <v>46</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F70" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G70" s="18" t="s">
+        <v>47</v>
+      </c>
       <c r="H70" s="13">
         <v>45.0</v>
       </c>
@@ -2811,24 +2920,24 @@
         <v>class-attribute-type-66</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="E71" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="F71" s="24" t="s">
-        <v>183</v>
-      </c>
-      <c r="G71" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="H71" s="17">
+        <v>185</v>
+      </c>
+      <c r="E71" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="F71" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="G71" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="H71" s="16">
         <v>66.0</v>
       </c>
     </row>
@@ -2838,24 +2947,24 @@
         <v>class-name-67</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D72" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E72" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="F72" s="26" t="s">
-        <v>186</v>
-      </c>
-      <c r="G72" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="H72" s="27">
+      <c r="E72" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="F72" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="G72" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="H72" s="25">
         <v>67.0</v>
       </c>
     </row>
@@ -2865,7 +2974,7 @@
         <v>connectors-with-same-name-multiplicity-68</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C73" s="15" t="s">
         <v>16</v>
@@ -2873,16 +2982,16 @@
       <c r="D73" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E73" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="F73" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="G73" s="24" t="s">
-        <v>191</v>
-      </c>
-      <c r="H73" s="28">
+      <c r="E73" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="F73" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="G73" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="H73" s="26">
         <v>68.0</v>
       </c>
     </row>
@@ -2892,24 +3001,24 @@
         <v>connectors-with-same-name-definition-69</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="D74" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E74" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="F74" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="G74" s="26" t="s">
-        <v>195</v>
-      </c>
-      <c r="H74" s="27">
+      <c r="E74" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="F74" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="G74" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="H74" s="25">
         <v>69.0</v>
       </c>
     </row>
@@ -2919,24 +3028,24 @@
         <v>connectors-with-same-name-definition-70</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="E75" s="24" t="s">
-        <v>193</v>
-      </c>
-      <c r="F75" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="G75" s="24" t="s">
-        <v>195</v>
-      </c>
-      <c r="H75" s="28">
+        <v>185</v>
+      </c>
+      <c r="E75" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="F75" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="G75" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="H75" s="26">
         <v>70.0</v>
       </c>
     </row>
@@ -2946,24 +3055,24 @@
         <v>class-attributes-with-same-name-definition-71</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="D76" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E76" s="26" t="s">
+      <c r="E76" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="F76" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="F76" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="G76" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="H76" s="27">
+      <c r="G76" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="H76" s="25">
         <v>71.0</v>
       </c>
     </row>
@@ -2973,7 +3082,7 @@
         <v>class-attributes-with-same-name-multiplicity-72</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C77" s="15" t="s">
         <v>16</v>
@@ -2981,16 +3090,16 @@
       <c r="D77" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E77" s="24" t="s">
-        <v>200</v>
-      </c>
-      <c r="F77" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="G77" s="24" t="s">
-        <v>201</v>
-      </c>
-      <c r="H77" s="28">
+      <c r="E77" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="F77" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="G77" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="H77" s="26">
         <v>72.0</v>
       </c>
     </row>
@@ -3000,24 +3109,24 @@
         <v>class-attributes-with-same-name-data-types-73</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="D78" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E78" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="F78" s="26" t="s">
-        <v>204</v>
-      </c>
-      <c r="G78" s="26" t="s">
-        <v>205</v>
-      </c>
-      <c r="H78" s="27">
+      <c r="E78" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="F78" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="G78" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="H78" s="25">
         <v>73.0</v>
       </c>
     </row>
@@ -12273,26 +12382,10 @@
     </row>
   </sheetData>
   <autoFilter ref="$A$7:$H$72"/>
-  <mergeCells count="19">
+  <mergeCells count="3">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A5:F5"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D57:G57"/>
-    <mergeCell ref="D58:G58"/>
-    <mergeCell ref="D59:G59"/>
-    <mergeCell ref="D69:G69"/>
-    <mergeCell ref="D70:G70"/>
-    <mergeCell ref="D24:G24"/>
-    <mergeCell ref="D25:G25"/>
-    <mergeCell ref="D26:G26"/>
-    <mergeCell ref="D47:G47"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="D51:G51"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>